<commit_message>
Bugfix suppression eleve + MàJ ref 2nde
</commit_message>
<xml_diff>
--- a/tables/Grille 2nde.xlsx
+++ b/tables/Grille 2nde.xlsx
@@ -4,16 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="17880" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="8175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Identification projet" sheetId="1" r:id="rId1"/>
-    <sheet name="Notation Candidat" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil1" sheetId="9" r:id="rId3"/>
+    <sheet name="Evaluation" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Evaluation!$A$1:$K$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Identification projet'!$A$1:$B$48</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Notation Candidat'!$A$1:$K$41</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="82">
   <si>
     <t>Identifications</t>
   </si>
@@ -146,36 +145,6 @@
     <t>Appréciation globale</t>
   </si>
   <si>
-    <t xml:space="preserve">C5.1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Préparer la solution et le plan d’action </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C5.2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mettre en œuvre une solution matérielle/logicielle en situation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C5.3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Effectuer la recette d’un produit avec le client </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C5.4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installer un système d’exploitation et/ou une bibliothèque logicielle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C5.5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Installer un dispositif de correction et/ou mise à jour de logiciel </t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -197,9 +166,6 @@
     <t>CO3.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Acquérir les bases d'une culture de l'innovation </t>
-  </si>
-  <si>
     <t>Mettre en œuvre une démarche de créativité</t>
   </si>
   <si>
@@ -209,97 +175,112 @@
     <t>Titre</t>
   </si>
   <si>
-    <t>relier les évolutions technologiques aux innovations qui marquent des ruptures dans les solutions techniques</t>
-  </si>
-  <si>
-    <t>utiliser un vocabulaire spécifique à l'innovation et la créativité</t>
-  </si>
-  <si>
-    <t>Identifier les principes qui régissent la propriété intellectuelle, la normalisation et l'intelligence économique</t>
-  </si>
-  <si>
-    <t>analyser le cycle de vie d'un produit</t>
-  </si>
-  <si>
-    <t>analyser l'impact environnemental d'un objet et de ses constituants</t>
-  </si>
-  <si>
-    <t>formuler des hypothèses, hierarchiser, sélectionner, expliciter, contextualiser</t>
-  </si>
-  <si>
-    <t>mettre en œuvre une ou des méthodes de créativité</t>
-  </si>
-  <si>
-    <t>matérialiser une solution innovante</t>
-  </si>
-  <si>
-    <t>Design et significations</t>
-  </si>
-  <si>
-    <t>Associer un objet à une grande période de la conception, des arts aux design industriel</t>
-  </si>
-  <si>
-    <t>Observer un objet d'un point de vue description, communication et représentation</t>
-  </si>
-  <si>
-    <t>Identifier un contexte (culturel, écologique, économique, sociétal, technologique)</t>
-  </si>
-  <si>
-    <t>Identifier des fonctions de besoins et d'usages</t>
-  </si>
-  <si>
     <t>Mettre en œuvre une démarche de création</t>
   </si>
   <si>
-    <t>Concevoir, réaliser, un projet de design, individuel ou collectif</t>
-  </si>
-  <si>
-    <t>confronter intension et réalisation dans la conduite d'un projet pour l'adapter et l'orienter, s'assurer de la dimension créative</t>
-  </si>
-  <si>
-    <t>faire preuve d'autonomie, d'initiative, d'engagement et d'esprit critique dans la conduite du projet</t>
-  </si>
-  <si>
-    <t>mener à terme une production individuelle dans le cadre d'un projet</t>
-  </si>
-  <si>
     <t>Approfondir la culture technologique</t>
   </si>
   <si>
-    <t>Identifier des contraintes associées à une norme</t>
-  </si>
-  <si>
-    <t>identifier la dimension sensible ou esthétique</t>
-  </si>
-  <si>
-    <t>identifier les fonctions d'un système technique</t>
-  </si>
-  <si>
-    <t>Identifier matériaux, flux d'énergie et d'information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">décrire la relation produit/matériau/procédé </t>
-  </si>
-  <si>
-    <t>exprimer une réflexion, un principe, une idée, une solution technique</t>
-  </si>
-  <si>
-    <t>exprimer sa pensée à l'aide d'outils de description adaptés, manuels ou numériques</t>
-  </si>
-  <si>
-    <t>Décrire, en utilisant les outils et les languages de descriptions adaptés</t>
-  </si>
-  <si>
-    <t>Interpréter des résultats expérimentaux, en tirer une conclusion et la communiquer en argumentant</t>
-  </si>
-  <si>
-    <t>Modéliser, simuler numériquement la structure et/ou le comportement d'un objet</t>
-  </si>
-  <si>
-    <t>CO3.2</t>
-  </si>
-  <si>
     <t>Candidat</t>
+  </si>
+  <si>
+    <t>Approfondir la culture design</t>
+  </si>
+  <si>
+    <t>Un objet est associé à une grande période de la conception, des arts aux design industriel</t>
+  </si>
+  <si>
+    <t>un objet est observé d'un point de vue description, communication et représentation</t>
+  </si>
+  <si>
+    <t>Le contexte est identifié (culturel, écologique, économique, sociétal, technologique)</t>
+  </si>
+  <si>
+    <t>Les fonctions de besoins et d'usages sont identifiées</t>
+  </si>
+  <si>
+    <t>Le projet de design, individuel ou collectif est conçu et réalisé</t>
+  </si>
+  <si>
+    <t>Intention et réalisation sont confrontées dans la conduite d'un projet pour l'adapter et l'orienter, la dimension créative est présente</t>
+  </si>
+  <si>
+    <t>Le projet est conduit de manière autonome avec initiative, engagement et esprit critique</t>
+  </si>
+  <si>
+    <t>la production individuelle dans le cadre d'un projet est conduite à son terme</t>
+  </si>
+  <si>
+    <t>Des contraintes associées à une norme sont identifiées</t>
+  </si>
+  <si>
+    <t>La dimension sensible ou esthétique est identifiée</t>
+  </si>
+  <si>
+    <t>Les fonctions d'un système technique sont identifiées</t>
+  </si>
+  <si>
+    <t>Les matériaux, flux d'énergie et d'information sont identifiés</t>
+  </si>
+  <si>
+    <t>Les grandeurs sont mesurées de manière directe ou indirecte</t>
+  </si>
+  <si>
+    <t>Les résultats expérimentaux sont interprétés, une conclusion est formulée</t>
+  </si>
+  <si>
+    <t>La structure et/ou le comportement d'un objet est simulée numériquement</t>
+  </si>
+  <si>
+    <t>Les évolutions technologiques sont reliées aux innovations qui marquent des ruptures dans les solutions techniques</t>
+  </si>
+  <si>
+    <t>Le vocabulaire spécifique à l'innovation et à la créativité est utilisé</t>
+  </si>
+  <si>
+    <t>Les principes qui régissent la propriété intellectuelle, la normalisation et l'intelligence économique sont identifiés</t>
+  </si>
+  <si>
+    <t>L'analyse du  cycle de vie d'un produit est réalisée</t>
+  </si>
+  <si>
+    <t>L'analyse de l'impact environnemental d'un objet et de ses constituants est réalisée</t>
+  </si>
+  <si>
+    <t>Acquérir les bases d'une culture de l'innovation technologique</t>
+  </si>
+  <si>
+    <t>Les hypothèses sont formulées, hiérarchisées, sélectionnées, explicitées, contextualisées</t>
+  </si>
+  <si>
+    <t>Une ou des méthodes de créativité sont mise en œuvre</t>
+  </si>
+  <si>
+    <t>Une solution innovante est matérialisée</t>
+  </si>
+  <si>
+    <t>Une réflexion, un principe, une idée, une solution technique sont exprimées</t>
+  </si>
+  <si>
+    <t>La pensée est exprimée à l'aide d'outils de description adaptés, manuels ou numériques</t>
+  </si>
+  <si>
+    <t>Les outils et les langages sont adaptés à la description</t>
+  </si>
+  <si>
+    <t>Les résultats expérimentaux sont interprétés, une conclusion argumentée est formulée et communiquée</t>
+  </si>
+  <si>
+    <t>Le vocabulaire spécifique à l'innovation et la créativité est utilisé</t>
+  </si>
+  <si>
+    <t>Simuler, mesurer un comportement</t>
+  </si>
+  <si>
+    <t>CO1.3</t>
+  </si>
+  <si>
+    <t>CO2.3</t>
   </si>
 </sst>
 </file>
@@ -458,12 +439,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Verdana"/>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,12 +463,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -537,7 +514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -767,84 +744,6 @@
       <top/>
       <bottom style="medium">
         <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1156,28 +1055,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1222,7 +1099,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1427,35 +1304,26 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1463,26 +1331,38 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1497,40 +1377,40 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1538,42 +1418,36 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1584,51 +1458,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -2142,17 +1989,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="82"/>
+      <c r="A1" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="83"/>
     </row>
     <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2163,7 +2010,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B4" s="7"/>
     </row>
@@ -2198,10 +2045,10 @@
       <c r="B9" s="11"/>
     </row>
     <row r="10" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="83" t="s">
-        <v>87</v>
-      </c>
-      <c r="B10" s="83"/>
+      <c r="A10" s="84" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="84"/>
     </row>
     <row r="11" spans="1:3" ht="18.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
@@ -2216,96 +2063,96 @@
       <c r="B12" s="12"/>
     </row>
     <row r="13" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="84"/>
+      <c r="B13" s="85"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="86"/>
-      <c r="B14" s="86"/>
+      <c r="A14" s="87"/>
+      <c r="B14" s="87"/>
       <c r="C14" s="13"/>
     </row>
     <row r="15" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="86"/>
-      <c r="B15" s="86"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="87"/>
     </row>
     <row r="16" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
+      <c r="A16" s="87"/>
+      <c r="B16" s="87"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="86"/>
-      <c r="B17" s="86"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="87"/>
     </row>
     <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="86"/>
-      <c r="B18" s="86"/>
+      <c r="A18" s="87"/>
+      <c r="B18" s="87"/>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="86"/>
-      <c r="B19" s="86"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="87"/>
     </row>
     <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="86"/>
-      <c r="B20" s="86"/>
+      <c r="A20" s="87"/>
+      <c r="B20" s="87"/>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="86"/>
-      <c r="B21" s="86"/>
+      <c r="A21" s="87"/>
+      <c r="B21" s="87"/>
     </row>
     <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="84" t="s">
+      <c r="A22" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="84"/>
+      <c r="B22" s="85"/>
       <c r="C22" s="13"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="87"/>
-      <c r="B23" s="87"/>
+      <c r="A23" s="88"/>
+      <c r="B23" s="88"/>
       <c r="C23" s="13"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="87"/>
-      <c r="B24" s="87"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="88"/>
       <c r="C24" s="13"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="87"/>
-      <c r="B25" s="87"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="88"/>
       <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="87"/>
-      <c r="B26" s="87"/>
+      <c r="A26" s="88"/>
+      <c r="B26" s="88"/>
       <c r="C26" s="13"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="87"/>
-      <c r="B27" s="87"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="88"/>
       <c r="C27" s="13"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="87"/>
-      <c r="B28" s="87"/>
+      <c r="A28" s="88"/>
+      <c r="B28" s="88"/>
       <c r="C28" s="13"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="87"/>
-      <c r="B29" s="87"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="88"/>
       <c r="C29" s="13"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="87"/>
-      <c r="B30" s="87"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="88"/>
       <c r="C30" s="13"/>
     </row>
     <row r="31" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="84" t="s">
+      <c r="A31" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="84"/>
+      <c r="B31" s="85"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
@@ -2315,8 +2162,8 @@
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="88"/>
-      <c r="B32" s="88"/>
+      <c r="A32" s="89"/>
+      <c r="B32" s="89"/>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
@@ -2326,8 +2173,8 @@
       <c r="I32" s="13"/>
     </row>
     <row r="33" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="88"/>
-      <c r="B33" s="88"/>
+      <c r="A33" s="89"/>
+      <c r="B33" s="89"/>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
@@ -2337,8 +2184,8 @@
       <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="88"/>
-      <c r="B34" s="88"/>
+      <c r="A34" s="89"/>
+      <c r="B34" s="89"/>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
@@ -2348,8 +2195,8 @@
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="88"/>
-      <c r="B35" s="88"/>
+      <c r="A35" s="89"/>
+      <c r="B35" s="89"/>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
@@ -2359,8 +2206,8 @@
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="88"/>
-      <c r="B36" s="88"/>
+      <c r="A36" s="89"/>
+      <c r="B36" s="89"/>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
@@ -2369,8 +2216,8 @@
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="88"/>
-      <c r="B37" s="88"/>
+      <c r="A37" s="89"/>
+      <c r="B37" s="89"/>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
@@ -2379,8 +2226,8 @@
       <c r="I37" s="13"/>
     </row>
     <row r="38" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="88"/>
-      <c r="B38" s="88"/>
+      <c r="A38" s="89"/>
+      <c r="B38" s="89"/>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
@@ -2389,8 +2236,8 @@
       <c r="I38" s="13"/>
     </row>
     <row r="39" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="88"/>
-      <c r="B39" s="88"/>
+      <c r="A39" s="89"/>
+      <c r="B39" s="89"/>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="13"/>
@@ -2399,10 +2246,10 @@
       <c r="I39" s="13"/>
     </row>
     <row r="40" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="84" t="s">
+      <c r="A40" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="84"/>
+      <c r="B40" s="85"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="13"/>
@@ -2411,8 +2258,8 @@
       <c r="I40" s="13"/>
     </row>
     <row r="41" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="85"/>
-      <c r="B41" s="85"/>
+      <c r="A41" s="86"/>
+      <c r="B41" s="86"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
@@ -2421,8 +2268,8 @@
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="85"/>
-      <c r="B42" s="85"/>
+      <c r="A42" s="86"/>
+      <c r="B42" s="86"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
       <c r="F42" s="13"/>
@@ -2431,8 +2278,8 @@
       <c r="I42" s="13"/>
     </row>
     <row r="43" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="85"/>
-      <c r="B43" s="85"/>
+      <c r="A43" s="86"/>
+      <c r="B43" s="86"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
       <c r="F43" s="13"/>
@@ -2441,8 +2288,8 @@
       <c r="I43" s="13"/>
     </row>
     <row r="44" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="85"/>
-      <c r="B44" s="85"/>
+      <c r="A44" s="86"/>
+      <c r="B44" s="86"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
@@ -2451,8 +2298,8 @@
       <c r="I44" s="13"/>
     </row>
     <row r="45" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="85"/>
-      <c r="B45" s="85"/>
+      <c r="A45" s="86"/>
+      <c r="B45" s="86"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
@@ -2461,8 +2308,8 @@
       <c r="I45" s="13"/>
     </row>
     <row r="46" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="85"/>
-      <c r="B46" s="85"/>
+      <c r="A46" s="86"/>
+      <c r="B46" s="86"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
       <c r="F46" s="13"/>
@@ -2471,8 +2318,8 @@
       <c r="I46" s="13"/>
     </row>
     <row r="47" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="85"/>
-      <c r="B47" s="85"/>
+      <c r="A47" s="86"/>
+      <c r="B47" s="86"/>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
@@ -2481,8 +2328,8 @@
       <c r="I47" s="13"/>
     </row>
     <row r="48" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="85"/>
-      <c r="B48" s="85"/>
+      <c r="A48" s="86"/>
+      <c r="B48" s="86"/>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
       <c r="F48" s="13"/>
@@ -2492,6 +2339,8 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B48"/>
     <mergeCell ref="A13:B13"/>
@@ -2500,8 +2349,6 @@
     <mergeCell ref="A23:B30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B39"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.74027777777777781" right="0.54027777777777775" top="0.70972222222222225" bottom="0.67986111111111103" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -2522,10 +2369,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC49"/>
+  <dimension ref="A1:AC52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2577,16 +2424,16 @@
       <c r="C2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="89" t="str">
+      <c r="D2" s="90" t="str">
         <f>IF('Identification projet'!B11="","Renseigner feuille Identification projet",'Identification projet'!B11)</f>
         <v>Renseigner feuille Identification projet</v>
       </c>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
       <c r="L2" s="54"/>
       <c r="M2" s="54"/>
       <c r="N2" s="55"/>
@@ -2610,16 +2457,16 @@
       <c r="C3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="89" t="str">
+      <c r="D3" s="90" t="str">
         <f>IF('Identification projet'!B12="","Renseigner feuille Identification projet",'Identification projet'!B12)</f>
         <v>Renseigner feuille Identification projet</v>
       </c>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
       <c r="K3" s="47"/>
       <c r="L3" s="59" t="s">
         <v>16</v>
@@ -2646,29 +2493,29 @@
       <c r="X3" s="58"/>
     </row>
     <row r="4" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="74" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="72">
-        <v>0</v>
-      </c>
-      <c r="F4" s="72" t="s">
+      <c r="E4" s="71">
+        <v>0</v>
+      </c>
+      <c r="F4" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="69"/>
+      <c r="I4" s="68"/>
       <c r="K4" s="34" t="s">
         <v>16</v>
       </c>
@@ -2713,21 +2560,21 @@
       </c>
     </row>
     <row r="5" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="120" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="121"/>
-      <c r="C5" s="75" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="107"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="69"/>
-      <c r="K5" s="70">
-        <v>0.2</v>
+      <c r="A5" s="119" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="120"/>
+      <c r="C5" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="108"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="68"/>
+      <c r="K5" s="69">
+        <v>0.15</v>
       </c>
       <c r="L5" s="49">
         <f>SUM(L6:L10)</f>
@@ -2751,18 +2598,18 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="98"/>
-      <c r="B6" s="99"/>
-      <c r="C6" s="80" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
+      <c r="A6" s="99"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
       <c r="I6" s="36" t="str">
-        <f t="shared" ref="I6:I16" si="0">(IF(W6&lt;&gt;0,"◄",""))</f>
+        <f t="shared" ref="I6:I22" si="0">(IF(W6&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
       <c r="J6" s="37"/>
@@ -2771,15 +2618,15 @@
         <v>1</v>
       </c>
       <c r="L6" s="60">
-        <f t="shared" ref="L6:L16" si="1">K6*S6</f>
+        <f t="shared" ref="L6:L22" si="1">K6*S6</f>
         <v>0</v>
       </c>
       <c r="M6" s="51">
-        <f t="shared" ref="M6:M16" si="2">S6*K6*20</f>
+        <f t="shared" ref="M6:M22" si="2">S6*K6*20</f>
         <v>0</v>
       </c>
       <c r="N6" s="51">
-        <f t="shared" ref="N6:N16" si="3">(IF(F6&lt;&gt;"",1/3,0)+IF(G6&lt;&gt;"",2/3,0)+IF(H6&lt;&gt;"",1,0))*K6*20</f>
+        <f t="shared" ref="N6:N22" si="3">(IF(F6&lt;&gt;"",1/3,0)+IF(G6&lt;&gt;"",2/3,0)+IF(H6&lt;&gt;"",1,0))*K6*20</f>
         <v>0</v>
       </c>
       <c r="O6" s="51" t="e">
@@ -2799,43 +2646,43 @@
         <v>#REF!</v>
       </c>
       <c r="S6" s="50">
-        <f t="shared" ref="S6:S16" si="4">IF(D6="",IF(E6&lt;&gt;"",1,0)+IF(F6&lt;&gt;"",1,0)+IF(G6&lt;&gt;"",1,0)+IF(H6&lt;&gt;"",1,0),0)</f>
+        <f t="shared" ref="S6:S22" si="4">IF(D6="",IF(E6&lt;&gt;"",1,0)+IF(F6&lt;&gt;"",1,0)+IF(G6&lt;&gt;"",1,0)+IF(H6&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="T6" s="52">
-        <f t="shared" ref="T6:T16" si="5">IF(D6&lt;&gt;"",0,(IF(E6&lt;&gt;"",0.02,(N6/(K6*20)))))</f>
+        <f t="shared" ref="T6:T22" si="5">IF(D6&lt;&gt;"",0,(IF(E6&lt;&gt;"",0.02,(N6/(K6*20)))))</f>
         <v>0</v>
       </c>
       <c r="U6" s="52">
-        <f t="shared" ref="U6:U16" si="6">IF(S6=0,0,K6)</f>
+        <f t="shared" ref="U6:U22" si="6">IF(S6=0,0,K6)</f>
         <v>0</v>
       </c>
       <c r="V6" s="64">
-        <f t="shared" ref="V6:V16" si="7">IF(D6&lt;&gt;"",IF(E6&lt;&gt;"",1,0)+IF(F6&lt;&gt;"",1,0)+IF(G6&lt;&gt;"",1,0)+IF(H6&lt;&gt;"",1,0),0)</f>
+        <f t="shared" ref="V6:V22" si="7">IF(D6&lt;&gt;"",IF(E6&lt;&gt;"",1,0)+IF(F6&lt;&gt;"",1,0)+IF(G6&lt;&gt;"",1,0)+IF(H6&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="W6" s="53">
-        <f t="shared" ref="W6:W16" si="8">IF(OR(S6&gt;1,V6&gt;0,AND(D6="",S6=0)),1,0)</f>
+        <f t="shared" ref="W6:W22" si="8">IF(OR(S6&gt;1,V6&gt;0,AND(D6="",S6=0)),1,0)</f>
         <v>1</v>
       </c>
       <c r="X6" s="53" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="Y6" s="33" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="98"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="78" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="78"/>
+      <c r="A7" s="99"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
       <c r="I7" s="36" t="str">
         <f t="shared" ref="I7:I10" si="9">(IF(W7&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
@@ -2894,23 +2741,23 @@
         <v>1</v>
       </c>
       <c r="X7" s="53" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="Y7" s="33" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="98"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="80" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
       <c r="I8" s="36" t="str">
         <f t="shared" si="9"/>
         <v>◄</v>
@@ -2969,23 +2816,23 @@
         <v>1</v>
       </c>
       <c r="X8" s="53" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="Y8" s="33" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="98"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="78" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
       <c r="I9" s="36" t="str">
         <f t="shared" si="9"/>
         <v>◄</v>
@@ -3044,23 +2891,23 @@
         <v>1</v>
       </c>
       <c r="X9" s="53" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="Y9" s="33" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="80" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
+      <c r="A10" s="99"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
       <c r="I10" s="36" t="str">
         <f t="shared" si="9"/>
         <v>◄</v>
@@ -3119,708 +2966,729 @@
         <v>1</v>
       </c>
       <c r="X10" s="53" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="Y10" s="33" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A11" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="97"/>
-      <c r="C11" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="93"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="95"/>
+      <c r="A11" s="97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="98"/>
+      <c r="C11" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="101"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="103"/>
       <c r="I11" s="36" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J11" s="37"/>
-      <c r="K11" s="70">
-        <v>0.2</v>
+      <c r="K11" s="69">
+        <v>0.15</v>
       </c>
       <c r="L11" s="60">
-        <f>SUM(L12:L14)</f>
+        <f>SUM(L12:L15)</f>
         <v>0</v>
       </c>
       <c r="M11" s="51"/>
       <c r="P11" s="51">
-        <f>SUM(P12:P14)</f>
+        <f>SUM(P12:P15)</f>
         <v>0</v>
       </c>
       <c r="S11" s="50">
-        <f>SUM(S12:S14)</f>
+        <f>SUM(S12:S15)</f>
         <v>0</v>
       </c>
       <c r="T11" s="62"/>
       <c r="V11" s="64"/>
       <c r="W11" s="53">
-        <f>SUM(W12:W14)</f>
-        <v>3</v>
+        <f>SUM(W12:W15)</f>
+        <v>4</v>
       </c>
       <c r="X11" s="53">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="98"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
+    <row r="12" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="99"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
       <c r="I12" s="36" t="str">
+        <f>(IF(W12&lt;&gt;0,"◄",""))</f>
+        <v>◄</v>
+      </c>
+      <c r="J12" s="37"/>
+      <c r="K12" s="48">
+        <f>IF(D12="",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="60">
+        <f>K12*S12</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="51">
+        <f>S12*K12*20</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="51">
+        <f>(IF(F12&lt;&gt;"",1/3,0)+IF(G12&lt;&gt;"",2/3,0)+IF(H12&lt;&gt;"",1,0))*K12*20</f>
+        <v>0</v>
+      </c>
+      <c r="O12" s="51" t="e">
+        <f>IF(#REF!=0,0,M12/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P12" s="51">
+        <f>IF($T$11=0,0,N12/$L$11)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="51" t="e">
+        <f>O12*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R12" s="51" t="e">
+        <f>P12*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S12" s="50">
+        <f>IF(D12="",IF(E12&lt;&gt;"",1,0)+IF(F12&lt;&gt;"",1,0)+IF(G12&lt;&gt;"",1,0)+IF(H12&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="52">
+        <f>IF(D12&lt;&gt;"",0,(IF(E12&lt;&gt;"",0.02,(N12/(K12*20)))))</f>
+        <v>0</v>
+      </c>
+      <c r="U12" s="52">
+        <f>IF(S12=0,0,K12)</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="64">
+        <f>IF(D12&lt;&gt;"",IF(E12&lt;&gt;"",1,0)+IF(F12&lt;&gt;"",1,0)+IF(G12&lt;&gt;"",1,0)+IF(H12&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W12" s="53">
+        <f>IF(OR(S12&gt;1,V12&gt;0,AND(D12="",S12=0)),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="99"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="36" t="str">
+        <f t="shared" ref="I13:I15" si="20">(IF(W13&lt;&gt;0,"◄",""))</f>
+        <v>◄</v>
+      </c>
+      <c r="J13" s="37"/>
+      <c r="K13" s="48">
+        <f t="shared" ref="K13:K15" si="21">IF(D13="",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="60">
+        <f t="shared" ref="L13:L15" si="22">K13*S13</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="51">
+        <f t="shared" ref="M13:M15" si="23">S13*K13*20</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="51">
+        <f t="shared" ref="N13:N15" si="24">(IF(F13&lt;&gt;"",1/3,0)+IF(G13&lt;&gt;"",2/3,0)+IF(H13&lt;&gt;"",1,0))*K13*20</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="51" t="e">
+        <f>IF(#REF!=0,0,M13/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P13" s="51">
+        <f>IF($T$11=0,0,N13/$L$11)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="51" t="e">
+        <f>O13*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R13" s="51" t="e">
+        <f>P13*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S13" s="50">
+        <f t="shared" ref="S13:S15" si="25">IF(D13="",IF(E13&lt;&gt;"",1,0)+IF(F13&lt;&gt;"",1,0)+IF(G13&lt;&gt;"",1,0)+IF(H13&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="52">
+        <f t="shared" ref="T13:T15" si="26">IF(D13&lt;&gt;"",0,(IF(E13&lt;&gt;"",0.02,(N13/(K13*20)))))</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="52">
+        <f t="shared" ref="U13:U15" si="27">IF(S13=0,0,K13)</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="64">
+        <f t="shared" ref="V13:V15" si="28">IF(D13&lt;&gt;"",IF(E13&lt;&gt;"",1,0)+IF(F13&lt;&gt;"",1,0)+IF(G13&lt;&gt;"",1,0)+IF(H13&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="53">
+        <f t="shared" ref="W13:W15" si="29">IF(OR(S13&gt;1,V13&gt;0,AND(D13="",S13=0)),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="99"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="36" t="str">
+        <f t="shared" si="20"/>
+        <v>◄</v>
+      </c>
+      <c r="J14" s="37"/>
+      <c r="K14" s="48">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="L14" s="60">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="51">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="51">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="51" t="e">
+        <f>IF(#REF!=0,0,M14/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P14" s="51">
+        <f>IF($T$11=0,0,N14/$L$11)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="51" t="e">
+        <f>O14*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R14" s="51" t="e">
+        <f>P14*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S14" s="50">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="T14" s="52">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="52">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="V14" s="64">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="W14" s="53">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="99"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="36" t="str">
+        <f t="shared" si="20"/>
+        <v>◄</v>
+      </c>
+      <c r="J15" s="37"/>
+      <c r="K15" s="48">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="L15" s="60">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="51">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="N15" s="51">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="51" t="e">
+        <f>IF(#REF!=0,0,M15/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P15" s="51">
+        <f>IF($T$11=0,0,N15/$L$11)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="51" t="e">
+        <f>O15*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R15" s="51" t="e">
+        <f>P15*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S15" s="50">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="52">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="52">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="V15" s="64">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="W15" s="53">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="97" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="98"/>
+      <c r="C16" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="116"/>
+      <c r="E16" s="117"/>
+      <c r="F16" s="117"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="37"/>
+      <c r="K16" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="L16" s="60">
+        <f>SUM(L20:L20)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="51"/>
+      <c r="P16" s="51">
+        <f>SUM(P20:P20)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="50">
+        <f>SUM(S17:S20)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="62"/>
+      <c r="V16" s="64"/>
+      <c r="W16" s="53">
+        <f>SUM(W20:W20)</f>
+        <v>1</v>
+      </c>
+      <c r="X16" s="53">
+        <v>4</v>
+      </c>
+      <c r="AA16" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="36" t="str">
+        <f>(IF(W17&lt;&gt;0,"◄",""))</f>
+        <v>◄</v>
+      </c>
+      <c r="J17" s="37"/>
+      <c r="K17" s="48">
+        <f>IF(D17="",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L17" s="60">
+        <f>K17*S17</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="51">
+        <f>S17*K17*20</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="51">
+        <f>(IF(F17&lt;&gt;"",1/3,0)+IF(G17&lt;&gt;"",2/3,0)+IF(H17&lt;&gt;"",1,0))*K17*20</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="51" t="e">
+        <f>IF(#REF!=0,0,M17/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P17" s="51">
+        <f>IF($T$16=0,0,N17/$L$16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="51" t="e">
+        <f>O17*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R17" s="51" t="e">
+        <f>P17*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S17" s="50">
+        <f>IF(D17="",IF(E17&lt;&gt;"",1,0)+IF(F17&lt;&gt;"",1,0)+IF(G17&lt;&gt;"",1,0)+IF(H17&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="52">
+        <f>IF(D17&lt;&gt;"",0,(IF(E17&lt;&gt;"",0.02,(N17/(K17*20)))))</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="52">
+        <f>IF(S17=0,0,K17)</f>
+        <v>0</v>
+      </c>
+      <c r="V17" s="64">
+        <f>IF(D17&lt;&gt;"",IF(E17&lt;&gt;"",1,0)+IF(F17&lt;&gt;"",1,0)+IF(G17&lt;&gt;"",1,0)+IF(H17&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W17" s="53">
+        <f>IF(OR(S17&gt;1,V17&gt;0,AND(D17="",S17=0)),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="99"/>
+      <c r="B18" s="100"/>
+      <c r="C18" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="36" t="str">
+        <f t="shared" ref="I18:I20" si="30">(IF(W18&lt;&gt;0,"◄",""))</f>
+        <v>◄</v>
+      </c>
+      <c r="J18" s="37"/>
+      <c r="K18" s="48">
+        <f t="shared" ref="K18:K20" si="31">IF(D18="",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="L18" s="60">
+        <f t="shared" ref="L18:L20" si="32">K18*S18</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="51">
+        <f t="shared" ref="M18:M20" si="33">S18*K18*20</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="51">
+        <f t="shared" ref="N18:N20" si="34">(IF(F18&lt;&gt;"",1/3,0)+IF(G18&lt;&gt;"",2/3,0)+IF(H18&lt;&gt;"",1,0))*K18*20</f>
+        <v>0</v>
+      </c>
+      <c r="O18" s="51" t="e">
+        <f>IF(#REF!=0,0,M18/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P18" s="51">
+        <f>IF($T$16=0,0,N18/$L$16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="51" t="e">
+        <f>O18*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R18" s="51" t="e">
+        <f>P18*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S18" s="50">
+        <f t="shared" ref="S18:S20" si="35">IF(D18="",IF(E18&lt;&gt;"",1,0)+IF(F18&lt;&gt;"",1,0)+IF(G18&lt;&gt;"",1,0)+IF(H18&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T18" s="52">
+        <f t="shared" ref="T18:T20" si="36">IF(D18&lt;&gt;"",0,(IF(E18&lt;&gt;"",0.02,(N18/(K18*20)))))</f>
+        <v>0</v>
+      </c>
+      <c r="U18" s="52">
+        <f t="shared" ref="U18:U20" si="37">IF(S18=0,0,K18)</f>
+        <v>0</v>
+      </c>
+      <c r="V18" s="64">
+        <f t="shared" ref="V18:V20" si="38">IF(D18&lt;&gt;"",IF(E18&lt;&gt;"",1,0)+IF(F18&lt;&gt;"",1,0)+IF(G18&lt;&gt;"",1,0)+IF(H18&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W18" s="53">
+        <f t="shared" ref="W18:W20" si="39">IF(OR(S18&gt;1,V18&gt;0,AND(D18="",S18=0)),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="99"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="36" t="str">
+        <f t="shared" si="30"/>
+        <v>◄</v>
+      </c>
+      <c r="J19" s="37"/>
+      <c r="K19" s="48">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="L19" s="60">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="51">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="51">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="51" t="e">
+        <f>IF(#REF!=0,0,M19/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P19" s="51">
+        <f>IF($T$16=0,0,N19/$L$16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="51" t="e">
+        <f>O19*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R19" s="51" t="e">
+        <f>P19*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S19" s="50">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="52">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="52">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="64">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="W19" s="53">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="99"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="74"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="36" t="str">
+        <f t="shared" si="30"/>
+        <v>◄</v>
+      </c>
+      <c r="J20" s="37"/>
+      <c r="K20" s="48">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="L20" s="60">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="51">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="51">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="51" t="e">
+        <f>IF(#REF!=0,0,M20/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P20" s="51">
+        <f>IF($T$16=0,0,N20/$L$16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="51" t="e">
+        <f>O20*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R20" s="51" t="e">
+        <f>P20*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S20" s="50">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="52">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="52">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="64">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="W20" s="53">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="Z20" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" s="97" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="98"/>
+      <c r="C21" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="94"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="95"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="37"/>
+      <c r="K21" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="L21" s="60">
+        <f>SUM(L22:L24)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="51"/>
+      <c r="P21" s="51">
+        <f>SUM(P22:P24)</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="50">
+        <f>SUM(S22:S24)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="62"/>
+      <c r="V21" s="64"/>
+      <c r="W21" s="53">
+        <f>SUM(W22:W24)</f>
+        <v>3</v>
+      </c>
+      <c r="X21" s="53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="99"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="77" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="36" t="str">
         <f t="shared" si="0"/>
         <v>◄</v>
       </c>
-      <c r="J12" s="37"/>
-      <c r="K12" s="48">
-        <f t="shared" ref="K12:K16" si="20">IF(D12="",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="L12" s="60">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="51">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N12" s="51">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O12" s="51" t="e">
-        <f>IF(#REF!=0,0,M12/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P12" s="51">
-        <f>IF($T$11=0,0,N12/$L$11)</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="51" t="e">
-        <f>O12*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R12" s="51" t="e">
-        <f>P12*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S12" s="50">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T12" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U12" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V12" s="64">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W12" s="53">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="98"/>
-      <c r="B13" s="99"/>
-      <c r="C13" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="36" t="str">
-        <f t="shared" ref="I13:I14" si="21">(IF(W13&lt;&gt;0,"◄",""))</f>
-        <v>◄</v>
-      </c>
-      <c r="J13" s="37"/>
-      <c r="K13" s="48">
-        <f t="shared" ref="K13:K14" si="22">IF(D13="",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="L13" s="60">
-        <f t="shared" ref="L13:L14" si="23">K13*S13</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="51">
-        <f t="shared" ref="M13:M14" si="24">S13*K13*20</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="51">
-        <f t="shared" ref="N13:N14" si="25">(IF(F13&lt;&gt;"",1/3,0)+IF(G13&lt;&gt;"",2/3,0)+IF(H13&lt;&gt;"",1,0))*K13*20</f>
-        <v>0</v>
-      </c>
-      <c r="O13" s="51" t="e">
-        <f>IF(#REF!=0,0,M13/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P13" s="51">
-        <f t="shared" ref="P13:P14" si="26">IF($T$11=0,0,N13/$L$11)</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="51" t="e">
-        <f>O13*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R13" s="51" t="e">
-        <f>P13*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S13" s="50">
-        <f t="shared" ref="S13:S14" si="27">IF(D13="",IF(E13&lt;&gt;"",1,0)+IF(F13&lt;&gt;"",1,0)+IF(G13&lt;&gt;"",1,0)+IF(H13&lt;&gt;"",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T13" s="52">
-        <f t="shared" ref="T13:T14" si="28">IF(D13&lt;&gt;"",0,(IF(E13&lt;&gt;"",0.02,(N13/(K13*20)))))</f>
-        <v>0</v>
-      </c>
-      <c r="U13" s="52">
-        <f t="shared" ref="U13:U14" si="29">IF(S13=0,0,K13)</f>
-        <v>0</v>
-      </c>
-      <c r="V13" s="64">
-        <f t="shared" ref="V13:V14" si="30">IF(D13&lt;&gt;"",IF(E13&lt;&gt;"",1,0)+IF(F13&lt;&gt;"",1,0)+IF(G13&lt;&gt;"",1,0)+IF(H13&lt;&gt;"",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="W13" s="53">
-        <f t="shared" ref="W13:W14" si="31">IF(OR(S13&gt;1,V13&gt;0,AND(D13="",S13=0)),1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A14" s="98"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="81" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="36" t="str">
-        <f t="shared" si="21"/>
-        <v>◄</v>
-      </c>
-      <c r="J14" s="37"/>
-      <c r="K14" s="48">
-        <f t="shared" si="22"/>
-        <v>1</v>
-      </c>
-      <c r="L14" s="60">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="51">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="51">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="51" t="e">
-        <f>IF(#REF!=0,0,M14/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P14" s="51">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="51" t="e">
-        <f>O14*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R14" s="51" t="e">
-        <f>P14*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S14" s="50">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="52">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="U14" s="52">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="V14" s="64">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="W14" s="53">
-        <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="96" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="97"/>
-      <c r="C15" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="117"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="119"/>
-      <c r="I15" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" s="37"/>
-      <c r="K15" s="70">
-        <v>0.2</v>
-      </c>
-      <c r="L15" s="60">
-        <f>SUM(L19:L19)</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="51"/>
-      <c r="P15" s="51">
-        <f>SUM(P19:P19)</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="50">
-        <f>SUM(S16:S19)</f>
-        <v>0</v>
-      </c>
-      <c r="T15" s="62"/>
-      <c r="V15" s="64"/>
-      <c r="W15" s="53">
-        <f>SUM(W19:W19)</f>
-        <v>1</v>
-      </c>
-      <c r="X15" s="53">
-        <v>4</v>
-      </c>
-      <c r="AA15" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="98"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="80" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="80"/>
-      <c r="E16" s="80"/>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>◄</v>
-      </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="48">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="L16" s="60">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="51">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="51">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="51" t="e">
-        <f>IF(#REF!=0,0,M16/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P16" s="51">
-        <f>IF($T$15=0,0,N16/$L$15)</f>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="51" t="e">
-        <f>O16*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R16" s="51" t="e">
-        <f>P16*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S16" s="50">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T16" s="52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U16" s="52">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V16" s="64">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="W16" s="53">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="98"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="36" t="str">
-        <f t="shared" ref="I17:I19" si="32">(IF(W17&lt;&gt;0,"◄",""))</f>
-        <v>◄</v>
-      </c>
-      <c r="J17" s="37"/>
-      <c r="K17" s="48">
-        <f t="shared" ref="K17:K19" si="33">IF(D17="",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="L17" s="60">
-        <f t="shared" ref="L17:L19" si="34">K17*S17</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="51">
-        <f t="shared" ref="M17:M19" si="35">S17*K17*20</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="51">
-        <f t="shared" ref="N17:N19" si="36">(IF(F17&lt;&gt;"",1/3,0)+IF(G17&lt;&gt;"",2/3,0)+IF(H17&lt;&gt;"",1,0))*K17*20</f>
-        <v>0</v>
-      </c>
-      <c r="O17" s="51" t="e">
-        <f>IF(#REF!=0,0,M17/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P17" s="51">
-        <f t="shared" ref="P17:P19" si="37">IF($T$15=0,0,N17/$L$15)</f>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="51" t="e">
-        <f>O17*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R17" s="51" t="e">
-        <f>P17*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S17" s="50">
-        <f t="shared" ref="S17:S19" si="38">IF(D17="",IF(E17&lt;&gt;"",1,0)+IF(F17&lt;&gt;"",1,0)+IF(G17&lt;&gt;"",1,0)+IF(H17&lt;&gt;"",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T17" s="52">
-        <f t="shared" ref="T17:T19" si="39">IF(D17&lt;&gt;"",0,(IF(E17&lt;&gt;"",0.02,(N17/(K17*20)))))</f>
-        <v>0</v>
-      </c>
-      <c r="U17" s="52">
-        <f t="shared" ref="U17:U19" si="40">IF(S17=0,0,K17)</f>
-        <v>0</v>
-      </c>
-      <c r="V17" s="64">
-        <f t="shared" ref="V17:V19" si="41">IF(D17&lt;&gt;"",IF(E17&lt;&gt;"",1,0)+IF(F17&lt;&gt;"",1,0)+IF(G17&lt;&gt;"",1,0)+IF(H17&lt;&gt;"",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="W17" s="53">
-        <f t="shared" ref="W17:W19" si="42">IF(OR(S17&gt;1,V17&gt;0,AND(D17="",S17=0)),1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="98"/>
-      <c r="B18" s="99"/>
-      <c r="C18" s="80" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
-      <c r="G18" s="80"/>
-      <c r="H18" s="80"/>
-      <c r="I18" s="36" t="str">
-        <f t="shared" si="32"/>
-        <v>◄</v>
-      </c>
-      <c r="J18" s="37"/>
-      <c r="K18" s="48">
-        <f t="shared" si="33"/>
-        <v>1</v>
-      </c>
-      <c r="L18" s="60">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="51">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="51" t="e">
-        <f>IF(#REF!=0,0,M18/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P18" s="51">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="51" t="e">
-        <f>O18*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R18" s="51" t="e">
-        <f>P18*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S18" s="50">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="T18" s="52">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="U18" s="52">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="V18" s="64">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="W18" s="53">
-        <f t="shared" si="42"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="98"/>
-      <c r="B19" s="99"/>
-      <c r="C19" s="78" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="36" t="str">
-        <f t="shared" si="32"/>
-        <v>◄</v>
-      </c>
-      <c r="J19" s="37"/>
-      <c r="K19" s="48">
-        <f t="shared" si="33"/>
-        <v>1</v>
-      </c>
-      <c r="L19" s="60">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="51">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="51" t="e">
-        <f>IF(#REF!=0,0,M19/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P19" s="51">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="51" t="e">
-        <f>O19*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R19" s="51" t="e">
-        <f>P19*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S19" s="50">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="52">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="U19" s="52">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="V19" s="64">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-      <c r="W19" s="53">
-        <f t="shared" si="42"/>
-        <v>1</v>
-      </c>
-      <c r="Z19" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="96" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="97"/>
-      <c r="C20" s="75" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="100"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="70">
-        <v>0.1</v>
-      </c>
-      <c r="L20" s="60"/>
-      <c r="M20" s="51"/>
-      <c r="V20" s="64"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="98"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="36" t="str">
-        <f t="shared" ref="I21" si="43">(IF(W21&lt;&gt;0,"◄",""))</f>
-        <v>◄</v>
-      </c>
-      <c r="J21" s="37"/>
-      <c r="K21" s="48">
-        <f t="shared" ref="K21" si="44">IF(D21="",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="L21" s="60">
-        <f t="shared" ref="L21" si="45">K21*S21</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="51">
-        <f t="shared" ref="M21" si="46">S21*K21*20</f>
-        <v>0</v>
-      </c>
-      <c r="N21" s="51">
-        <f t="shared" ref="N21" si="47">(IF(F21&lt;&gt;"",1/3,0)+IF(G21&lt;&gt;"",2/3,0)+IF(H21&lt;&gt;"",1,0))*K21*20</f>
-        <v>0</v>
-      </c>
-      <c r="O21" s="51" t="e">
-        <f>IF(#REF!=0,0,M21/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P21" s="51">
-        <f t="shared" ref="P21" si="48">IF($T$15=0,0,N21/$L$15)</f>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="51" t="e">
-        <f>O21*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R21" s="51" t="e">
-        <f>P21*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S21" s="50">
-        <f t="shared" ref="S21" si="49">IF(D21="",IF(E21&lt;&gt;"",1,0)+IF(F21&lt;&gt;"",1,0)+IF(G21&lt;&gt;"",1,0)+IF(H21&lt;&gt;"",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T21" s="52">
-        <f t="shared" ref="T21" si="50">IF(D21&lt;&gt;"",0,(IF(E21&lt;&gt;"",0.02,(N21/(K21*20)))))</f>
-        <v>0</v>
-      </c>
-      <c r="U21" s="52">
-        <f t="shared" ref="U21" si="51">IF(S21=0,0,K21)</f>
-        <v>0</v>
-      </c>
-      <c r="V21" s="64">
-        <f t="shared" ref="V21" si="52">IF(D21&lt;&gt;"",IF(E21&lt;&gt;"",1,0)+IF(F21&lt;&gt;"",1,0)+IF(G21&lt;&gt;"",1,0)+IF(H21&lt;&gt;"",1,0),0)</f>
-        <v>0</v>
-      </c>
-      <c r="W21" s="53">
-        <f t="shared" ref="W21" si="53">IF(OR(S21&gt;1,V21&gt;0,AND(D21="",S21=0)),1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" ht="24" x14ac:dyDescent="0.2">
-      <c r="A22" s="98"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="79" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="79"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="36" t="str">
-        <f t="shared" ref="I22:I24" si="54">(IF(W22&lt;&gt;0,"◄",""))</f>
-        <v>◄</v>
-      </c>
       <c r="J22" s="37"/>
       <c r="K22" s="48">
-        <f t="shared" ref="K22:K24" si="55">IF(D22="",1,0)</f>
+        <f t="shared" ref="K22" si="40">IF(D22="",1,0)</f>
         <v>1</v>
       </c>
       <c r="L22" s="60">
-        <f t="shared" ref="L22:L24" si="56">K22*S22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M22" s="51">
-        <f t="shared" ref="M22:M24" si="57">S22*K22*20</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N22" s="51">
-        <f t="shared" ref="N22:N24" si="58">(IF(F22&lt;&gt;"",1/3,0)+IF(G22&lt;&gt;"",2/3,0)+IF(H22&lt;&gt;"",1,0))*K22*20</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O22" s="51" t="e">
@@ -3828,7 +3696,7 @@
         <v>#REF!</v>
       </c>
       <c r="P22" s="51">
-        <f t="shared" ref="P22:P24" si="59">IF($T$15=0,0,N22/$L$15)</f>
+        <f>IF($T$21=0,0,N22/$L$21)</f>
         <v>0</v>
       </c>
       <c r="Q22" s="51" t="e">
@@ -3840,56 +3708,56 @@
         <v>#REF!</v>
       </c>
       <c r="S22" s="50">
-        <f t="shared" ref="S22:S24" si="60">IF(D22="",IF(E22&lt;&gt;"",1,0)+IF(F22&lt;&gt;"",1,0)+IF(G22&lt;&gt;"",1,0)+IF(H22&lt;&gt;"",1,0),0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T22" s="52">
-        <f t="shared" ref="T22:T24" si="61">IF(D22&lt;&gt;"",0,(IF(E22&lt;&gt;"",0.02,(N22/(K22*20)))))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U22" s="52">
-        <f t="shared" ref="U22:U24" si="62">IF(S22=0,0,K22)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V22" s="64">
-        <f t="shared" ref="V22:V24" si="63">IF(D22&lt;&gt;"",IF(E22&lt;&gt;"",1,0)+IF(F22&lt;&gt;"",1,0)+IF(G22&lt;&gt;"",1,0)+IF(H22&lt;&gt;"",1,0),0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W22" s="53">
-        <f t="shared" ref="W22:W24" si="64">IF(OR(S22&gt;1,V22&gt;0,AND(D22="",S22=0)),1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="98"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="81" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="99"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="36" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" ref="I23:I24" si="41">(IF(W23&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
       <c r="J23" s="37"/>
       <c r="K23" s="48">
-        <f t="shared" si="55"/>
+        <f t="shared" ref="K23:K24" si="42">IF(D23="",1,0)</f>
         <v>1</v>
       </c>
       <c r="L23" s="60">
-        <f t="shared" si="56"/>
+        <f t="shared" ref="L23:L24" si="43">K23*S23</f>
         <v>0</v>
       </c>
       <c r="M23" s="51">
-        <f t="shared" si="57"/>
+        <f t="shared" ref="M23:M24" si="44">S23*K23*20</f>
         <v>0</v>
       </c>
       <c r="N23" s="51">
-        <f t="shared" si="58"/>
+        <f t="shared" ref="N23:N24" si="45">(IF(F23&lt;&gt;"",1/3,0)+IF(G23&lt;&gt;"",2/3,0)+IF(H23&lt;&gt;"",1,0))*K23*20</f>
         <v>0</v>
       </c>
       <c r="O23" s="51" t="e">
@@ -3897,7 +3765,7 @@
         <v>#REF!</v>
       </c>
       <c r="P23" s="51">
-        <f t="shared" si="59"/>
+        <f t="shared" ref="P23:P24" si="46">IF($T$21=0,0,N23/$L$21)</f>
         <v>0</v>
       </c>
       <c r="Q23" s="51" t="e">
@@ -3909,56 +3777,56 @@
         <v>#REF!</v>
       </c>
       <c r="S23" s="50">
-        <f t="shared" si="60"/>
+        <f t="shared" ref="S23:S24" si="47">IF(D23="",IF(E23&lt;&gt;"",1,0)+IF(F23&lt;&gt;"",1,0)+IF(G23&lt;&gt;"",1,0)+IF(H23&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="T23" s="52">
-        <f t="shared" si="61"/>
+        <f t="shared" ref="T23:T24" si="48">IF(D23&lt;&gt;"",0,(IF(E23&lt;&gt;"",0.02,(N23/(K23*20)))))</f>
         <v>0</v>
       </c>
       <c r="U23" s="52">
-        <f t="shared" si="62"/>
+        <f t="shared" ref="U23:U24" si="49">IF(S23=0,0,K23)</f>
         <v>0</v>
       </c>
       <c r="V23" s="64">
-        <f t="shared" si="63"/>
+        <f t="shared" ref="V23:V24" si="50">IF(D23&lt;&gt;"",IF(E23&lt;&gt;"",1,0)+IF(F23&lt;&gt;"",1,0)+IF(G23&lt;&gt;"",1,0)+IF(H23&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="W23" s="53">
-        <f t="shared" si="64"/>
+        <f t="shared" ref="W23:W24" si="51">IF(OR(S23&gt;1,V23&gt;0,AND(D23="",S23=0)),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="98"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="81" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
+      <c r="A24" s="99"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
       <c r="I24" s="36" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="41"/>
         <v>◄</v>
       </c>
       <c r="J24" s="37"/>
       <c r="K24" s="48">
-        <f t="shared" si="55"/>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="L24" s="60">
-        <f t="shared" si="56"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="M24" s="51">
-        <f t="shared" si="57"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="N24" s="51">
-        <f t="shared" si="58"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="O24" s="51" t="e">
@@ -3966,7 +3834,7 @@
         <v>#REF!</v>
       </c>
       <c r="P24" s="51">
-        <f t="shared" si="59"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Q24" s="51" t="e">
@@ -3978,99 +3846,78 @@
         <v>#REF!</v>
       </c>
       <c r="S24" s="50">
-        <f t="shared" si="60"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="T24" s="52">
-        <f t="shared" si="61"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="U24" s="52">
-        <f t="shared" si="62"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="V24" s="64">
-        <f t="shared" si="63"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="W24" s="53">
-        <f t="shared" si="64"/>
+        <f t="shared" si="51"/>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="96" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="97"/>
-      <c r="C25" s="76" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="100"/>
-      <c r="E25" s="101"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
-      <c r="H25" s="102"/>
-      <c r="I25" s="36" t="s">
+      <c r="A25" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="98"/>
+      <c r="C25" s="81" t="s">
         <v>46</v>
       </c>
+      <c r="D25" s="101"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="103"/>
+      <c r="I25" s="36"/>
       <c r="J25" s="37"/>
-      <c r="K25" s="70">
-        <v>0.2</v>
-      </c>
-      <c r="L25" s="60">
-        <f>SUM(L26:L30)</f>
-        <v>0</v>
-      </c>
+      <c r="K25" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="L25" s="60"/>
       <c r="M25" s="51"/>
-      <c r="P25" s="51">
-        <f>SUM(P26:P30)</f>
-        <v>0</v>
-      </c>
-      <c r="S25" s="50">
-        <f>SUM(S26:S30)</f>
-        <v>0</v>
-      </c>
-      <c r="T25" s="62"/>
       <c r="V25" s="64"/>
-      <c r="W25" s="53">
-        <f>SUM(W26:W30)</f>
-        <v>5</v>
-      </c>
-      <c r="X25" s="53">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="98"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="80" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
-      <c r="G26" s="80"/>
-      <c r="H26" s="80"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="99"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
       <c r="I26" s="36" t="str">
-        <f t="shared" ref="I26:I32" si="65">(IF(W26&lt;&gt;0,"◄",""))</f>
+        <f t="shared" ref="I26" si="52">(IF(W26&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
       <c r="J26" s="37"/>
       <c r="K26" s="48">
-        <f>IF(D26="",1,0)</f>
+        <f t="shared" ref="K26" si="53">IF(D26="",1,0)</f>
         <v>1</v>
       </c>
       <c r="L26" s="60">
-        <f t="shared" ref="L26:L32" si="66">K26*S26</f>
+        <f t="shared" ref="L26" si="54">K26*S26</f>
         <v>0</v>
       </c>
       <c r="M26" s="51">
-        <f t="shared" ref="M26:M32" si="67">S26*K26*20</f>
+        <f t="shared" ref="M26" si="55">S26*K26*20</f>
         <v>0</v>
       </c>
       <c r="N26" s="51">
-        <f t="shared" ref="N26:N32" si="68">(IF(F26&lt;&gt;"",1/3,0)+IF(G26&lt;&gt;"",2/3,0)+IF(H26&lt;&gt;"",1,0))*K26*20</f>
+        <f t="shared" ref="N26" si="56">(IF(F26&lt;&gt;"",1/3,0)+IF(G26&lt;&gt;"",2/3,0)+IF(H26&lt;&gt;"",1,0))*K26*20</f>
         <v>0</v>
       </c>
       <c r="O26" s="51" t="e">
@@ -4078,7 +3925,7 @@
         <v>#REF!</v>
       </c>
       <c r="P26" s="51">
-        <f>IF($T$25=0,0,N26/$L$25)</f>
+        <f>IF($T$16=0,0,N26/$L$16)</f>
         <v>0</v>
       </c>
       <c r="Q26" s="51" t="e">
@@ -4090,56 +3937,56 @@
         <v>#REF!</v>
       </c>
       <c r="S26" s="50">
-        <f t="shared" ref="S26:S32" si="69">IF(D26="",IF(E26&lt;&gt;"",1,0)+IF(F26&lt;&gt;"",1,0)+IF(G26&lt;&gt;"",1,0)+IF(H26&lt;&gt;"",1,0),0)</f>
+        <f t="shared" ref="S26" si="57">IF(D26="",IF(E26&lt;&gt;"",1,0)+IF(F26&lt;&gt;"",1,0)+IF(G26&lt;&gt;"",1,0)+IF(H26&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="T26" s="52">
-        <f t="shared" ref="T26:T32" si="70">IF(D26&lt;&gt;"",0,(IF(E26&lt;&gt;"",0.02,(N26/(K26*20)))))</f>
+        <f t="shared" ref="T26" si="58">IF(D26&lt;&gt;"",0,(IF(E26&lt;&gt;"",0.02,(N26/(K26*20)))))</f>
         <v>0</v>
       </c>
       <c r="U26" s="52">
-        <f t="shared" ref="U26:U32" si="71">IF(S26=0,0,K26)</f>
+        <f t="shared" ref="U26" si="59">IF(S26=0,0,K26)</f>
         <v>0</v>
       </c>
       <c r="V26" s="64">
-        <f t="shared" ref="V26:V32" si="72">IF(D26&lt;&gt;"",IF(E26&lt;&gt;"",1,0)+IF(F26&lt;&gt;"",1,0)+IF(G26&lt;&gt;"",1,0)+IF(H26&lt;&gt;"",1,0),0)</f>
+        <f t="shared" ref="V26" si="60">IF(D26&lt;&gt;"",IF(E26&lt;&gt;"",1,0)+IF(F26&lt;&gt;"",1,0)+IF(G26&lt;&gt;"",1,0)+IF(H26&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="W26" s="53">
-        <f t="shared" ref="W26:W32" si="73">IF(OR(S26&gt;1,V26&gt;0,AND(D26="",S26=0)),1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="98"/>
-      <c r="B27" s="99"/>
-      <c r="C27" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
+        <f t="shared" ref="W26" si="61">IF(OR(S26&gt;1,V26&gt;0,AND(D26="",S26=0)),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="24" x14ac:dyDescent="0.2">
+      <c r="A27" s="99"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
       <c r="I27" s="36" t="str">
-        <f t="shared" ref="I27:I30" si="74">(IF(W27&lt;&gt;0,"◄",""))</f>
+        <f t="shared" ref="I27:I29" si="62">(IF(W27&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
       <c r="J27" s="37"/>
       <c r="K27" s="48">
-        <f t="shared" ref="K27:K30" si="75">IF(D27="",1,0)</f>
+        <f t="shared" ref="K27:K29" si="63">IF(D27="",1,0)</f>
         <v>1</v>
       </c>
       <c r="L27" s="60">
-        <f t="shared" ref="L27:L30" si="76">K27*S27</f>
+        <f t="shared" ref="L27:L29" si="64">K27*S27</f>
         <v>0</v>
       </c>
       <c r="M27" s="51">
-        <f t="shared" ref="M27:M30" si="77">S27*K27*20</f>
+        <f t="shared" ref="M27:M29" si="65">S27*K27*20</f>
         <v>0</v>
       </c>
       <c r="N27" s="51">
-        <f t="shared" ref="N27:N30" si="78">(IF(F27&lt;&gt;"",1/3,0)+IF(G27&lt;&gt;"",2/3,0)+IF(H27&lt;&gt;"",1,0))*K27*20</f>
+        <f t="shared" ref="N27:N29" si="66">(IF(F27&lt;&gt;"",1/3,0)+IF(G27&lt;&gt;"",2/3,0)+IF(H27&lt;&gt;"",1,0))*K27*20</f>
         <v>0</v>
       </c>
       <c r="O27" s="51" t="e">
@@ -4147,7 +3994,7 @@
         <v>#REF!</v>
       </c>
       <c r="P27" s="51">
-        <f t="shared" ref="P27:P30" si="79">IF($T$25=0,0,N27/$L$25)</f>
+        <f>IF($T$16=0,0,N27/$L$16)</f>
         <v>0</v>
       </c>
       <c r="Q27" s="51" t="e">
@@ -4159,56 +4006,56 @@
         <v>#REF!</v>
       </c>
       <c r="S27" s="50">
-        <f t="shared" ref="S27:S30" si="80">IF(D27="",IF(E27&lt;&gt;"",1,0)+IF(F27&lt;&gt;"",1,0)+IF(G27&lt;&gt;"",1,0)+IF(H27&lt;&gt;"",1,0),0)</f>
+        <f t="shared" ref="S27:S29" si="67">IF(D27="",IF(E27&lt;&gt;"",1,0)+IF(F27&lt;&gt;"",1,0)+IF(G27&lt;&gt;"",1,0)+IF(H27&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="T27" s="52">
-        <f t="shared" ref="T27:T30" si="81">IF(D27&lt;&gt;"",0,(IF(E27&lt;&gt;"",0.02,(N27/(K27*20)))))</f>
+        <f t="shared" ref="T27:T29" si="68">IF(D27&lt;&gt;"",0,(IF(E27&lt;&gt;"",0.02,(N27/(K27*20)))))</f>
         <v>0</v>
       </c>
       <c r="U27" s="52">
-        <f t="shared" ref="U27:U30" si="82">IF(S27=0,0,K27)</f>
+        <f t="shared" ref="U27:U29" si="69">IF(S27=0,0,K27)</f>
         <v>0</v>
       </c>
       <c r="V27" s="64">
-        <f t="shared" ref="V27:V30" si="83">IF(D27&lt;&gt;"",IF(E27&lt;&gt;"",1,0)+IF(F27&lt;&gt;"",1,0)+IF(G27&lt;&gt;"",1,0)+IF(H27&lt;&gt;"",1,0),0)</f>
+        <f t="shared" ref="V27:V29" si="70">IF(D27&lt;&gt;"",IF(E27&lt;&gt;"",1,0)+IF(F27&lt;&gt;"",1,0)+IF(G27&lt;&gt;"",1,0)+IF(H27&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="W27" s="53">
-        <f t="shared" ref="W27:W30" si="84">IF(OR(S27&gt;1,V27&gt;0,AND(D27="",S27=0)),1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="98"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="80"/>
+        <f t="shared" ref="W27:W29" si="71">IF(OR(S27&gt;1,V27&gt;0,AND(D27="",S27=0)),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28" s="99"/>
+      <c r="B28" s="100"/>
+      <c r="C28" s="77" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
       <c r="I28" s="36" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="62"/>
         <v>◄</v>
       </c>
       <c r="J28" s="37"/>
       <c r="K28" s="48">
-        <f t="shared" si="75"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="L28" s="60">
-        <f t="shared" si="76"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="M28" s="51">
-        <f t="shared" si="77"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="N28" s="51">
-        <f t="shared" si="78"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="O28" s="51" t="e">
@@ -4216,7 +4063,7 @@
         <v>#REF!</v>
       </c>
       <c r="P28" s="51">
-        <f t="shared" si="79"/>
+        <f>IF($T$16=0,0,N28/$L$16)</f>
         <v>0</v>
       </c>
       <c r="Q28" s="51" t="e">
@@ -4228,56 +4075,56 @@
         <v>#REF!</v>
       </c>
       <c r="S28" s="50">
-        <f t="shared" si="80"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="T28" s="52">
-        <f t="shared" si="81"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="U28" s="52">
-        <f t="shared" si="82"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="V28" s="64">
-        <f t="shared" si="83"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="W28" s="53">
-        <f t="shared" si="84"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="98"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="80"/>
-      <c r="H29" s="80"/>
+        <f t="shared" si="71"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="99"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
       <c r="I29" s="36" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="62"/>
         <v>◄</v>
       </c>
       <c r="J29" s="37"/>
       <c r="K29" s="48">
-        <f t="shared" si="75"/>
+        <f t="shared" si="63"/>
         <v>1</v>
       </c>
       <c r="L29" s="60">
-        <f t="shared" si="76"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="M29" s="51">
-        <f t="shared" si="77"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="N29" s="51">
-        <f t="shared" si="78"/>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="O29" s="51" t="e">
@@ -4285,7 +4132,7 @@
         <v>#REF!</v>
       </c>
       <c r="P29" s="51">
-        <f t="shared" si="79"/>
+        <f>IF($T$16=0,0,N29/$L$16)</f>
         <v>0</v>
       </c>
       <c r="Q29" s="51" t="e">
@@ -4297,168 +4144,147 @@
         <v>#REF!</v>
       </c>
       <c r="S29" s="50">
-        <f t="shared" si="80"/>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="T29" s="52">
-        <f t="shared" si="81"/>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="U29" s="52">
-        <f t="shared" si="82"/>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="V29" s="64">
-        <f t="shared" si="83"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="W29" s="53">
-        <f t="shared" si="84"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="110"/>
-      <c r="B30" s="111"/>
-      <c r="C30" s="78" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="78"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="36" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" si="71"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" s="97" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="98"/>
+      <c r="C30" s="81" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="101"/>
+      <c r="E30" s="102"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="102"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="69">
+        <v>0.15</v>
+      </c>
+      <c r="L30" s="60"/>
+      <c r="M30" s="51"/>
+      <c r="V30" s="64"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="99"/>
+      <c r="B31" s="100"/>
+      <c r="C31" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="36" t="str">
+        <f t="shared" ref="I31:I33" si="72">(IF(W31&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
-      <c r="J30" s="37"/>
-      <c r="K30" s="48">
-        <f t="shared" si="75"/>
-        <v>1</v>
-      </c>
-      <c r="L30" s="60">
-        <f t="shared" si="76"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="51">
-        <f t="shared" si="77"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="51">
-        <f t="shared" si="78"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="51" t="e">
-        <f>IF(#REF!=0,0,M30/#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="P30" s="51">
-        <f t="shared" si="79"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="51" t="e">
-        <f>O30*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R30" s="51" t="e">
-        <f>P30*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="S30" s="50">
-        <f t="shared" si="80"/>
-        <v>0</v>
-      </c>
-      <c r="T30" s="52">
-        <f t="shared" si="81"/>
-        <v>0</v>
-      </c>
-      <c r="U30" s="52">
-        <f t="shared" si="82"/>
-        <v>0</v>
-      </c>
-      <c r="V30" s="64">
-        <f t="shared" si="83"/>
-        <v>0</v>
-      </c>
-      <c r="W30" s="53">
-        <f t="shared" si="84"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="96" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="97"/>
-      <c r="C31" s="77" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="114"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="115"/>
-      <c r="H31" s="116"/>
-      <c r="I31" s="36" t="s">
-        <v>46</v>
-      </c>
       <c r="J31" s="37"/>
-      <c r="K31" s="70">
-        <v>0.2</v>
+      <c r="K31" s="48">
+        <f t="shared" ref="K31:K33" si="73">IF(D31="",1,0)</f>
+        <v>1</v>
       </c>
       <c r="L31" s="60">
-        <f>SUM(L32:L36)</f>
-        <v>0</v>
-      </c>
-      <c r="M31" s="51"/>
+        <f t="shared" ref="L31:L33" si="74">K31*S31</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="51">
+        <f t="shared" ref="M31:M33" si="75">S31*K31*20</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="51">
+        <f t="shared" ref="N31:N33" si="76">(IF(F31&lt;&gt;"",1/3,0)+IF(G31&lt;&gt;"",2/3,0)+IF(H31&lt;&gt;"",1,0))*K31*20</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="51" t="e">
+        <f>IF(#REF!=0,0,M31/#REF!)</f>
+        <v>#REF!</v>
+      </c>
       <c r="P31" s="51">
-        <f>SUM(P32:P36)</f>
-        <v>0</v>
+        <f t="shared" ref="P31:P33" si="77">IF($T$5=0,0,N31/$L$5)</f>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="51" t="e">
+        <f>O31*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R31" s="51" t="e">
+        <f>P31*#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="S31" s="50">
-        <f>SUM(S32:S36)</f>
-        <v>0</v>
-      </c>
-      <c r="T31" s="62"/>
-      <c r="V31" s="64"/>
+        <f t="shared" ref="S31:S33" si="78">IF(D31="",IF(E31&lt;&gt;"",1,0)+IF(F31&lt;&gt;"",1,0)+IF(G31&lt;&gt;"",1,0)+IF(H31&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T31" s="52">
+        <f t="shared" ref="T31:T33" si="79">IF(D31&lt;&gt;"",0,(IF(E31&lt;&gt;"",0.02,(N31/(K31*20)))))</f>
+        <v>0</v>
+      </c>
+      <c r="U31" s="52">
+        <f t="shared" ref="U31:U33" si="80">IF(S31=0,0,K31)</f>
+        <v>0</v>
+      </c>
+      <c r="V31" s="64">
+        <f t="shared" ref="V31:V33" si="81">IF(D31&lt;&gt;"",IF(E31&lt;&gt;"",1,0)+IF(F31&lt;&gt;"",1,0)+IF(G31&lt;&gt;"",1,0)+IF(H31&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
       <c r="W31" s="53">
-        <f>SUM(W32:W36)</f>
-        <v>5</v>
-      </c>
-      <c r="X31" s="53">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="98"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="81" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="81"/>
-      <c r="E32" s="81"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="81"/>
+        <f t="shared" ref="W31:W33" si="82">IF(OR(S31&gt;1,V31&gt;0,AND(D31="",S31=0)),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A32" s="99"/>
+      <c r="B32" s="100"/>
+      <c r="C32" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
       <c r="I32" s="36" t="str">
-        <f t="shared" si="65"/>
+        <f t="shared" si="72"/>
         <v>◄</v>
       </c>
       <c r="J32" s="37"/>
       <c r="K32" s="48">
-        <f t="shared" ref="K32" si="85">IF(D32="",1,0)</f>
+        <f t="shared" si="73"/>
         <v>1</v>
       </c>
       <c r="L32" s="60">
-        <f t="shared" si="66"/>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="M32" s="51">
-        <f t="shared" si="67"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="N32" s="51">
-        <f t="shared" si="68"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="O32" s="51" t="e">
@@ -4466,7 +4292,7 @@
         <v>#REF!</v>
       </c>
       <c r="P32" s="51">
-        <f>IF($T$31=0,0,N32/$L$31)</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="Q32" s="51" t="e">
@@ -4478,56 +4304,56 @@
         <v>#REF!</v>
       </c>
       <c r="S32" s="50">
-        <f t="shared" si="69"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="T32" s="52">
-        <f t="shared" si="70"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="U32" s="52">
-        <f t="shared" si="71"/>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="V32" s="64">
+        <f t="shared" si="81"/>
+        <v>0</v>
+      </c>
+      <c r="W32" s="53">
+        <f t="shared" si="82"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A33" s="99"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="77" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="36" t="str">
         <f t="shared" si="72"/>
-        <v>0</v>
-      </c>
-      <c r="W32" s="53">
-        <f t="shared" si="73"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="98"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="36" t="str">
-        <f t="shared" ref="I33:I36" si="86">(IF(W33&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
       <c r="J33" s="37"/>
       <c r="K33" s="48">
-        <f t="shared" ref="K33:K36" si="87">IF(D33="",1,0)</f>
+        <f t="shared" si="73"/>
         <v>1</v>
       </c>
       <c r="L33" s="60">
-        <f t="shared" ref="L33:L36" si="88">K33*S33</f>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="M33" s="51">
-        <f t="shared" ref="M33:M36" si="89">S33*K33*20</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="N33" s="51">
-        <f t="shared" ref="N33:N36" si="90">(IF(F33&lt;&gt;"",1/3,0)+IF(G33&lt;&gt;"",2/3,0)+IF(H33&lt;&gt;"",1,0))*K33*20</f>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="O33" s="51" t="e">
@@ -4535,7 +4361,7 @@
         <v>#REF!</v>
       </c>
       <c r="P33" s="51">
-        <f t="shared" ref="P33:P36" si="91">IF($T$31=0,0,N33/$L$31)</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="Q33" s="51" t="e">
@@ -4547,125 +4373,99 @@
         <v>#REF!</v>
       </c>
       <c r="S33" s="50">
-        <f t="shared" ref="S33:S36" si="92">IF(D33="",IF(E33&lt;&gt;"",1,0)+IF(F33&lt;&gt;"",1,0)+IF(G33&lt;&gt;"",1,0)+IF(H33&lt;&gt;"",1,0),0)</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="T33" s="52">
-        <f t="shared" ref="T33:T36" si="93">IF(D33&lt;&gt;"",0,(IF(E33&lt;&gt;"",0.02,(N33/(K33*20)))))</f>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="U33" s="52">
-        <f t="shared" ref="U33:U36" si="94">IF(S33=0,0,K33)</f>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="V33" s="64">
-        <f t="shared" ref="V33:V36" si="95">IF(D33&lt;&gt;"",IF(E33&lt;&gt;"",1,0)+IF(F33&lt;&gt;"",1,0)+IF(G33&lt;&gt;"",1,0)+IF(H33&lt;&gt;"",1,0),0)</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="W33" s="53">
-        <f t="shared" ref="W33:W36" si="96">IF(OR(S33&gt;1,V33&gt;0,AND(D33="",S33=0)),1,0)</f>
+        <f t="shared" si="82"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="98"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="81" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="36" t="str">
-        <f t="shared" si="86"/>
-        <v>◄</v>
+      <c r="A34" s="97" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="98"/>
+      <c r="C34" s="82" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="113"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="114"/>
+      <c r="G34" s="114"/>
+      <c r="H34" s="115"/>
+      <c r="I34" s="36" t="s">
+        <v>36</v>
       </c>
       <c r="J34" s="37"/>
-      <c r="K34" s="48">
-        <f t="shared" si="87"/>
-        <v>1</v>
+      <c r="K34" s="69">
+        <v>0.1</v>
       </c>
       <c r="L34" s="60">
-        <f t="shared" si="88"/>
-        <v>0</v>
-      </c>
-      <c r="M34" s="51">
-        <f t="shared" si="89"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="51">
-        <f t="shared" si="90"/>
-        <v>0</v>
-      </c>
-      <c r="O34" s="51" t="e">
-        <f>IF(#REF!=0,0,M34/#REF!)</f>
-        <v>#REF!</v>
-      </c>
+        <f>SUM(L35:L39)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="51"/>
       <c r="P34" s="51">
-        <f t="shared" si="91"/>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="51" t="e">
-        <f>O34*#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="R34" s="51" t="e">
-        <f>P34*#REF!</f>
-        <v>#REF!</v>
+        <f>SUM(P35:P39)</f>
+        <v>0</v>
       </c>
       <c r="S34" s="50">
-        <f t="shared" si="92"/>
-        <v>0</v>
-      </c>
-      <c r="T34" s="52">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="U34" s="52">
-        <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="V34" s="64">
-        <f t="shared" si="95"/>
-        <v>0</v>
-      </c>
+        <f>SUM(S35:S39)</f>
+        <v>0</v>
+      </c>
+      <c r="T34" s="62"/>
+      <c r="V34" s="64"/>
       <c r="W34" s="53">
-        <f t="shared" si="96"/>
-        <v>1</v>
+        <f>SUM(W35:W39)</f>
+        <v>5</v>
+      </c>
+      <c r="X34" s="53">
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="98"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="81" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
       <c r="I35" s="36" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" ref="I35" si="83">(IF(W35&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
       <c r="J35" s="37"/>
       <c r="K35" s="48">
-        <f t="shared" si="87"/>
+        <f t="shared" ref="K35" si="84">IF(D35="",1,0)</f>
         <v>1</v>
       </c>
       <c r="L35" s="60">
-        <f t="shared" si="88"/>
+        <f t="shared" ref="L35" si="85">K35*S35</f>
         <v>0</v>
       </c>
       <c r="M35" s="51">
-        <f t="shared" si="89"/>
+        <f t="shared" ref="M35" si="86">S35*K35*20</f>
         <v>0</v>
       </c>
       <c r="N35" s="51">
-        <f t="shared" si="90"/>
+        <f t="shared" ref="N35" si="87">(IF(F35&lt;&gt;"",1/3,0)+IF(G35&lt;&gt;"",2/3,0)+IF(H35&lt;&gt;"",1,0))*K35*20</f>
         <v>0</v>
       </c>
       <c r="O35" s="51" t="e">
@@ -4673,7 +4473,7 @@
         <v>#REF!</v>
       </c>
       <c r="P35" s="51">
-        <f t="shared" si="91"/>
+        <f>IF($T$34=0,0,N35/$L$34)</f>
         <v>0</v>
       </c>
       <c r="Q35" s="51" t="e">
@@ -4685,56 +4485,56 @@
         <v>#REF!</v>
       </c>
       <c r="S35" s="50">
-        <f t="shared" si="92"/>
+        <f t="shared" ref="S35" si="88">IF(D35="",IF(E35&lt;&gt;"",1,0)+IF(F35&lt;&gt;"",1,0)+IF(G35&lt;&gt;"",1,0)+IF(H35&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="T35" s="52">
-        <f t="shared" si="93"/>
+        <f t="shared" ref="T35" si="89">IF(D35&lt;&gt;"",0,(IF(E35&lt;&gt;"",0.02,(N35/(K35*20)))))</f>
         <v>0</v>
       </c>
       <c r="U35" s="52">
-        <f t="shared" si="94"/>
+        <f t="shared" ref="U35" si="90">IF(S35=0,0,K35)</f>
         <v>0</v>
       </c>
       <c r="V35" s="64">
-        <f t="shared" si="95"/>
+        <f t="shared" ref="V35" si="91">IF(D35&lt;&gt;"",IF(E35&lt;&gt;"",1,0)+IF(F35&lt;&gt;"",1,0)+IF(G35&lt;&gt;"",1,0)+IF(H35&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="W35" s="53">
-        <f t="shared" si="96"/>
+        <f t="shared" ref="W35" si="92">IF(OR(S35&gt;1,V35&gt;0,AND(D35="",S35=0)),1,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="112"/>
-      <c r="B36" s="113"/>
-      <c r="C36" s="79" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="79"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
+      <c r="A36" s="99"/>
+      <c r="B36" s="100"/>
+      <c r="C36" s="74" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
       <c r="I36" s="36" t="str">
-        <f t="shared" si="86"/>
+        <f t="shared" ref="I36:I39" si="93">(IF(W36&lt;&gt;0,"◄",""))</f>
         <v>◄</v>
       </c>
       <c r="J36" s="37"/>
       <c r="K36" s="48">
-        <f t="shared" si="87"/>
+        <f t="shared" ref="K36:K39" si="94">IF(D36="",1,0)</f>
         <v>1</v>
       </c>
       <c r="L36" s="60">
-        <f t="shared" si="88"/>
+        <f t="shared" ref="L36:L39" si="95">K36*S36</f>
         <v>0</v>
       </c>
       <c r="M36" s="51">
-        <f t="shared" si="89"/>
+        <f t="shared" ref="M36:M39" si="96">S36*K36*20</f>
         <v>0</v>
       </c>
       <c r="N36" s="51">
-        <f t="shared" si="90"/>
+        <f t="shared" ref="N36:N39" si="97">(IF(F36&lt;&gt;"",1/3,0)+IF(G36&lt;&gt;"",2/3,0)+IF(H36&lt;&gt;"",1,0))*K36*20</f>
         <v>0</v>
       </c>
       <c r="O36" s="51" t="e">
@@ -4742,7 +4542,7 @@
         <v>#REF!</v>
       </c>
       <c r="P36" s="51">
-        <f t="shared" si="91"/>
+        <f t="shared" ref="P36:P39" si="98">IF($T$34=0,0,N36/$L$34)</f>
         <v>0</v>
       </c>
       <c r="Q36" s="51" t="e">
@@ -4754,157 +4554,370 @@
         <v>#REF!</v>
       </c>
       <c r="S36" s="50">
-        <f t="shared" si="92"/>
+        <f t="shared" ref="S36:S39" si="99">IF(D36="",IF(E36&lt;&gt;"",1,0)+IF(F36&lt;&gt;"",1,0)+IF(G36&lt;&gt;"",1,0)+IF(H36&lt;&gt;"",1,0),0)</f>
         <v>0</v>
       </c>
       <c r="T36" s="52">
+        <f t="shared" ref="T36:T39" si="100">IF(D36&lt;&gt;"",0,(IF(E36&lt;&gt;"",0.02,(N36/(K36*20)))))</f>
+        <v>0</v>
+      </c>
+      <c r="U36" s="52">
+        <f t="shared" ref="U36:U39" si="101">IF(S36=0,0,K36)</f>
+        <v>0</v>
+      </c>
+      <c r="V36" s="64">
+        <f t="shared" ref="V36:V39" si="102">IF(D36&lt;&gt;"",IF(E36&lt;&gt;"",1,0)+IF(F36&lt;&gt;"",1,0)+IF(G36&lt;&gt;"",1,0)+IF(H36&lt;&gt;"",1,0),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W36" s="53">
+        <f t="shared" ref="W36:W39" si="103">IF(OR(S36&gt;1,V36&gt;0,AND(D36="",S36=0)),1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="99"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="36" t="str">
         <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
-      <c r="U36" s="52">
+        <v>◄</v>
+      </c>
+      <c r="J37" s="37"/>
+      <c r="K37" s="48">
         <f t="shared" si="94"/>
-        <v>0</v>
-      </c>
-      <c r="V36" s="64">
+        <v>1</v>
+      </c>
+      <c r="L37" s="60">
         <f t="shared" si="95"/>
         <v>0</v>
       </c>
-      <c r="W36" s="53">
+      <c r="M37" s="51">
         <f t="shared" si="96"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="38"/>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
-      <c r="G37" s="92"/>
-      <c r="H37" s="92"/>
-      <c r="I37" s="36"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="65"/>
-      <c r="S37" s="61"/>
-      <c r="U37" s="66"/>
-      <c r="V37" s="67"/>
-      <c r="W37" s="63"/>
-      <c r="X37" s="61"/>
-    </row>
-    <row r="38" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="103" t="str">
-        <f>(IF(W37&gt;0,"ATTENTION. Erreur de saisie : cocher une seule colonne par ligne ! Voir repères ◄ à droite de la grille.",""))</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="51">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="O37" s="51" t="e">
+        <f>IF(#REF!=0,0,M37/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P37" s="51">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="51" t="e">
+        <f>O37*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R37" s="51" t="e">
+        <f>P37*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S37" s="50">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="T37" s="52">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="U37" s="52">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="V37" s="64">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+      <c r="W37" s="53">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="99"/>
+      <c r="B38" s="100"/>
+      <c r="C38" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="36" t="str">
+        <f t="shared" si="93"/>
+        <v>◄</v>
+      </c>
+      <c r="J38" s="37"/>
+      <c r="K38" s="48">
+        <f t="shared" si="94"/>
+        <v>1</v>
+      </c>
+      <c r="L38" s="60">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="51">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="51">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="O38" s="51" t="e">
+        <f>IF(#REF!=0,0,M38/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P38" s="51">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="51" t="e">
+        <f>O38*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R38" s="51" t="e">
+        <f>P38*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S38" s="50">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="T38" s="52">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="U38" s="52">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="V38" s="64">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+      <c r="W38" s="53">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="111"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="36" t="str">
+        <f t="shared" si="93"/>
+        <v>◄</v>
+      </c>
+      <c r="J39" s="37"/>
+      <c r="K39" s="48">
+        <f t="shared" si="94"/>
+        <v>1</v>
+      </c>
+      <c r="L39" s="60">
+        <f t="shared" si="95"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="51">
+        <f t="shared" si="96"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="51">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="51" t="e">
+        <f>IF(#REF!=0,0,M39/#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P39" s="51">
+        <f t="shared" si="98"/>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="51" t="e">
+        <f>O39*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="R39" s="51" t="e">
+        <f>P39*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S39" s="50">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="52">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="U39" s="52">
+        <f t="shared" si="101"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="64">
+        <f t="shared" si="102"/>
+        <v>0</v>
+      </c>
+      <c r="W39" s="53">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="38"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="93"/>
+      <c r="H40" s="93"/>
+      <c r="I40" s="36"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="65"/>
+      <c r="S40" s="61"/>
+      <c r="U40" s="66"/>
+      <c r="V40" s="67"/>
+      <c r="W40" s="63"/>
+      <c r="X40" s="61"/>
+    </row>
+    <row r="41" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="104" t="str">
+        <f>(IF(W40&gt;0,"ATTENTION. Erreur de saisie : cocher une seule colonne par ligne ! Voir repères ◄ à droite de la grille.",""))</f>
         <v/>
       </c>
-      <c r="D38" s="103"/>
-      <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
-      <c r="G38" s="103"/>
-      <c r="H38" s="103"/>
-      <c r="I38" s="39" t="s">
+      <c r="D41" s="104"/>
+      <c r="E41" s="104"/>
+      <c r="F41" s="104"/>
+      <c r="G41" s="104"/>
+      <c r="H41" s="104"/>
+      <c r="I41" s="39" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="104" t="s">
+      <c r="K41" s="22">
+        <f>SUM(K5,K11,K16,K21,K25,K30,K34)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="104"/>
-      <c r="C39" s="105"/>
-      <c r="D39" s="105"/>
-      <c r="E39" s="105"/>
-      <c r="F39" s="105"/>
-      <c r="G39" s="105"/>
-      <c r="H39" s="105"/>
-      <c r="I39" s="41"/>
-    </row>
-    <row r="40" spans="1:24" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="106"/>
-      <c r="B40" s="106"/>
-      <c r="C40" s="106"/>
-      <c r="D40" s="106"/>
-      <c r="E40" s="106"/>
-      <c r="F40" s="106"/>
-      <c r="G40" s="106"/>
-      <c r="H40" s="106"/>
-      <c r="I40" s="42"/>
-    </row>
-    <row r="41" spans="1:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="42"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="44"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="45"/>
-    </row>
-    <row r="43" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="129">
-        <f>W37</f>
-        <v>0</v>
-      </c>
-      <c r="B43" s="46"/>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A44" s="130">
+      <c r="B42" s="105"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="106"/>
+      <c r="E42" s="106"/>
+      <c r="F42" s="106"/>
+      <c r="G42" s="106"/>
+      <c r="H42" s="106"/>
+      <c r="I42" s="41"/>
+    </row>
+    <row r="43" spans="1:24" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="107"/>
+      <c r="B43" s="107"/>
+      <c r="C43" s="107"/>
+      <c r="D43" s="107"/>
+      <c r="E43" s="107"/>
+      <c r="F43" s="107"/>
+      <c r="G43" s="107"/>
+      <c r="H43" s="107"/>
+      <c r="I43" s="42"/>
+    </row>
+    <row r="44" spans="1:24" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="42"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="45"/>
+    </row>
+    <row r="46" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="78">
+        <f>W40</f>
+        <v>0</v>
+      </c>
+      <c r="B46" s="46"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A47" s="79">
         <f>W5</f>
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A45" s="130">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A48" s="79">
+        <f>W21</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="78">
+        <f>W16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="78">
         <f>W11</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A46" s="129">
-        <f>W15</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A47" s="129">
-        <f>W25</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="78">
+        <f>W34</f>
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A48" s="129">
-        <f>W31</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="129">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="78">
         <f>W6</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="A40:H40"/>
+  <mergeCells count="22">
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="A43:H43"/>
     <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A25:B30"/>
-    <mergeCell ref="A31:B36"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="A11:B15"/>
+    <mergeCell ref="A34:B39"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D16:H16"/>
     <mergeCell ref="A5:B10"/>
-    <mergeCell ref="A15:B19"/>
-    <mergeCell ref="A11:B14"/>
+    <mergeCell ref="A16:B20"/>
+    <mergeCell ref="A21:B24"/>
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A20:B24"/>
-    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="A25:B29"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="A30:B33"/>
+    <mergeCell ref="D30:H30"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -4919,197 +4932,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D6:G24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:G17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D6" s="122"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="123"/>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D7" s="122"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="123"/>
-    </row>
-    <row r="8" spans="4:7" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="125" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="125" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="125" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="125" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D9" s="126"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
-    </row>
-    <row r="10" spans="4:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="125" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="125" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="125" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="125" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D11" s="126"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="126"/>
-    </row>
-    <row r="12" spans="4:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D12" s="125" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="125" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="125" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="125" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D13" s="126"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="126"/>
-    </row>
-    <row r="14" spans="4:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="127"/>
-      <c r="E14" s="127"/>
-      <c r="F14" s="125" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="125" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D15" s="128"/>
-      <c r="E15" s="128"/>
-      <c r="F15" s="126"/>
-      <c r="G15" s="126"/>
-    </row>
-    <row r="16" spans="4:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
-      <c r="F16" s="125" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="125" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D17" s="128"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="126"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D18" s="122"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="123"/>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D21" s="68"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="68"/>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-    </row>
-  </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>